<commit_message>
refactoring ans code clean
</commit_message>
<xml_diff>
--- a/tests/data/missing_master.xlsx
+++ b/tests/data/missing_master.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sax/Documents/data/PROGETTI/UNICEF/hope-smart-import/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C21F8F31-6C2F-0644-9885-D90D89D90D5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{681F3948-B394-7F42-A68D-D562FEF7FBF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4127,8 +4127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O103"/>
   <sheetViews>
-    <sheetView topLeftCell="A86" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A104" sqref="A104"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A87" sqref="A87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8969,7 +8969,7 @@
   <dimension ref="A1:R371"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="148" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>